<commit_message>
update dashboard, Dispatch, Inventory, History
</commit_message>
<xml_diff>
--- a/ex/Book1.xlsx
+++ b/ex/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Project\ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D4A9BA-22D8-42B3-B93E-55A5C62527D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FB01BE-4F5E-409A-8CDA-D2D4BF17A8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D6C18F03-564A-40AA-A193-15F4CED7891A}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>Sale Part</t>
   </si>
   <si>
-    <t>ให้โชว์ข้อมูล Dashboard  ซึ่งจะกลายเป็นหน้าแรกโชว์ข้อมูล 5 ช่อง ช่องที่1 โชว์ยอดออเดอร์ที่ต้องส่ง ช่องที่2 โชว์ว่าวันนี้ส่งไปแล้วกี่ออเดอร์ ช่องที่3 โชว์ว่าวันนี้ยังไม่ได้ส่งกี่ออเดอร์ ช่องที่4 โชว์ว่ายอดที่ Delay หรือยอดค้างของเมื่อวานที่ต้องส่งเท่าไหร่ ช่องที่5 โชว์ว่ายอดที่ต้องส่ง+ยอดค้างส่งแล้ะข้างล่างให้โชว์ข้อมูลในตาม format ใน Excel ที่ทำเป็นตัวอย่างให้ดู</t>
+    <t>ให้โชว์ข้อมูล Dashboard  ซึ่งจะกลายเป็นหน้าแรกโชว์ข้อมูล 5 ช่อง ช่องที่1 โชว์ยอดออเดอร์ที่ต้องส่งทั้งหมด500ต่อวัน ช่องที่2 โชว์ว่าวันนี้ส่งไปแล้วกี่ออเดอร์ ช่องที่3 โชว์ว่าวันนี้ยังไม่ได้ส่งกี่ออเดอร์ ช่องที่4 โชว์ว่ายอดที่ Delay หรือยอดค้างของเมื่อวานที่ต้องส่งเท่าไหร่ ช่องที่5 โชว์ว่ายอดที่ต้องส่ง+ยอดค้างส่งแล้ะข้างล่างให้โชว์ข้อมูลในตาม format ใน Excel ที่ทำเป็นตัวอย่างให้ดู</t>
   </si>
 </sst>
 </file>
@@ -136,10 +136,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,28 +491,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
@@ -522,7 +522,7 @@
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -541,13 +541,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>